<commit_message>
transcription error with Bodega Ridge orcs (#98)
xlsx file changes only
</commit_message>
<xml_diff>
--- a/migrations-data/20221102211341_data.xlsx
+++ b/migrations-data/20221102211341_data.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">0473</t>
   </si>
   <si>
-    <t xml:space="preserve">9954</t>
+    <t xml:space="preserve">9554</t>
   </si>
   <si>
     <t xml:space="preserve">Bodega Ridge Park</t>
@@ -238,7 +238,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>